<commit_message>
#update format formula excel and ui
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Account_Template.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountPayable/AP_Account_Template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
   <si>
     <t>{CompanyName}</t>
   </si>
@@ -144,43 +144,58 @@
     <t>{GiamTotal}</t>
   </si>
   <si>
+    <t>{RemainDt}</t>
+  </si>
+  <si>
+    <t>{RemainVndGrp}</t>
+  </si>
+  <si>
+    <t>{RemainVndTotal}</t>
+  </si>
+  <si>
+    <t>{RemainVndDt}</t>
+  </si>
+  <si>
+    <t>{BeginAmountVndGrp}</t>
+  </si>
+  <si>
+    <t>{BeginAmountVndDt}</t>
+  </si>
+  <si>
+    <t>{BeginAmountVndTotal}</t>
+  </si>
+  <si>
+    <t>{TangVndDt}</t>
+  </si>
+  <si>
+    <t>{TangVndTotal}</t>
+  </si>
+  <si>
+    <t>{GiamVndDt}</t>
+  </si>
+  <si>
+    <t>{GiamVndTotal}</t>
+  </si>
+  <si>
+    <t>{AccountGrp}</t>
+  </si>
+  <si>
+    <t>{TangGrp}</t>
+  </si>
+  <si>
+    <t>{GiamGrp}</t>
+  </si>
+  <si>
+    <t>{TangVndGrp}</t>
+  </si>
+  <si>
+    <t>{GiamVndGrp}</t>
+  </si>
+  <si>
     <t>{RemainGrp}</t>
   </si>
   <si>
-    <t>{RemainDt}</t>
-  </si>
-  <si>
     <t>{RemainTotal}</t>
-  </si>
-  <si>
-    <t>{RemainVndGrp}</t>
-  </si>
-  <si>
-    <t>{RemainVndTotal}</t>
-  </si>
-  <si>
-    <t>{RemainVndDt}</t>
-  </si>
-  <si>
-    <t>{BeginAmountVndGrp}</t>
-  </si>
-  <si>
-    <t>{BeginAmountVndDt}</t>
-  </si>
-  <si>
-    <t>{BeginAmountVndTotal}</t>
-  </si>
-  <si>
-    <t>{TangVndDt}</t>
-  </si>
-  <si>
-    <t>{TangVndTotal}</t>
-  </si>
-  <si>
-    <t>{GiamVndDt}</t>
-  </si>
-  <si>
-    <t>{GiamVndTotal}</t>
   </si>
 </sst>
 </file>
@@ -582,6 +597,36 @@
     <xf numFmtId="41" fontId="5" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -591,12 +636,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -605,30 +644,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -913,7 +928,10 @@
   <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <pane xSplit="7" ySplit="4" topLeftCell="H5" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,110 +952,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="33"/>
+      <c r="P1" s="33"/>
+      <c r="Q1" s="33"/>
+      <c r="R1" s="33"/>
     </row>
     <row r="2" spans="1:18" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="M2" s="34"/>
+      <c r="N2" s="34"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
+      <c r="R2" s="34"/>
     </row>
     <row r="3" spans="1:18" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
+      <c r="M3" s="35"/>
+      <c r="N3" s="35"/>
+      <c r="O3" s="35"/>
+      <c r="P3" s="35"/>
+      <c r="Q3" s="35"/>
+      <c r="R3" s="35"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="28"/>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="28"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="29"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="27" t="s">
+      <c r="B7" s="37"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="27"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="29" t="s">
         <v>8</v>
       </c>
       <c r="I7" s="31" t="s">
@@ -1049,25 +1067,25 @@
       <c r="K7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="L7" s="26" t="s">
+      <c r="L7" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="M7" s="26" t="s">
+      <c r="M7" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="N7" s="26" t="s">
+      <c r="N7" s="29" t="s">
         <v>14</v>
       </c>
       <c r="O7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="R7" s="26" t="s">
+      <c r="R7" s="29" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1088,18 +1106,18 @@
         <v>21</v>
       </c>
       <c r="F8" s="32"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
       <c r="I8" s="32"/>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="30"/>
       <c r="O8" s="32"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="30"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
@@ -1108,27 +1126,37 @@
       <c r="D9" s="6"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="33" t="s">
+      <c r="G9" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="34"/>
-      <c r="J9" s="35"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="25"/>
       <c r="K9" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L9" s="8"/>
-      <c r="M9" s="8"/>
+      <c r="L9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="M9" s="8" t="s">
+        <v>54</v>
+      </c>
       <c r="N9" s="8" t="s">
-        <v>41</v>
+        <v>57</v>
       </c>
       <c r="O9" s="20" t="s">
-        <v>47</v>
-      </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="20"/>
+        <v>45</v>
+      </c>
+      <c r="P9" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q9" s="20" t="s">
+        <v>56</v>
+      </c>
       <c r="R9" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
@@ -1172,19 +1200,19 @@
         <v>37</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="O10" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="P10" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="Q10" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="Q10" s="21" t="s">
-        <v>52</v>
-      </c>
       <c r="R10" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1195,11 +1223,11 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="37"/>
-      <c r="J11" s="38"/>
+      <c r="I11" s="27"/>
+      <c r="J11" s="28"/>
       <c r="K11" s="17" t="s">
         <v>38</v>
       </c>
@@ -1210,28 +1238,23 @@
         <v>40</v>
       </c>
       <c r="N11" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="R11" s="22" t="s">
         <v>43</v>
-      </c>
-      <c r="O11" s="22" t="s">
-        <v>49</v>
-      </c>
-      <c r="P11" s="22" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q11" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="R11" s="22" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="H11:J11"/>
-    <mergeCell ref="M7:M8"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="O7:O8"/>
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:R2"/>
     <mergeCell ref="A3:R3"/>
@@ -1248,6 +1271,11 @@
     <mergeCell ref="J7:J8"/>
     <mergeCell ref="K7:K8"/>
     <mergeCell ref="L7:L8"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="H11:J11"/>
+    <mergeCell ref="M7:M8"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="O7:O8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>